<commit_message>
More BOM and schematic cleanup
</commit_message>
<xml_diff>
--- a/pcb/denmark_bom.xlsx
+++ b/pcb/denmark_bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\STM32CubeIDE\workspace_1.11.0\denmark\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B3662F-8034-4E6A-8D94-9C31574DAF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E8B9BF-F3D5-411E-89C0-B84D8901298D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>Digikey P/N</t>
   </si>
@@ -104,9 +105,6 @@
     <t>497-STM32F401RET7-ND</t>
   </si>
   <si>
-    <t>U$1</t>
-  </si>
-  <si>
     <t>stm32f4 mcu</t>
   </si>
   <si>
@@ -327,6 +325,18 @@
   </si>
   <si>
     <t>296-SN74AHC1G08DBV3CT-ND</t>
+  </si>
+  <si>
+    <t>1727-2097-1-ND</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3v3 zener diode </t>
+  </si>
+  <si>
+    <t>U1</t>
   </si>
 </sst>
 </file>
@@ -607,7 +617,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -644,10 +654,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D32" si="0">B2*2</f>
+        <f t="shared" ref="D2:D33" si="0">B2*2</f>
         <v>20</v>
       </c>
       <c r="E2" t="s">
@@ -751,465 +761,482 @@
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
       </c>
       <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1">
         <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
         <v>35</v>
-      </c>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
       </c>
       <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
         <v>38</v>
-      </c>
-      <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
         <v>42</v>
-      </c>
-      <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E16" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
         <v>45</v>
-      </c>
-      <c r="D17" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
         <v>48</v>
-      </c>
-      <c r="D18" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
       <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
         <v>51</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E19" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
       <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
         <v>54</v>
-      </c>
-      <c r="D20" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1">
         <v>5</v>
       </c>
       <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
         <v>58</v>
-      </c>
-      <c r="D22" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="E22" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="1">
         <v>6</v>
       </c>
       <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
         <v>61</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="E23" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="1">
         <v>4</v>
       </c>
       <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
         <v>64</v>
-      </c>
-      <c r="D24" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
       <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
         <v>67</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
       </c>
       <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
         <v>70</v>
-      </c>
-      <c r="D26" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E26" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="1">
         <v>7</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28" s="1">
         <v>2</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B29" s="1">
         <v>2</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="1">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" x14ac:dyDescent="0.2"/>
-    <row r="34" x14ac:dyDescent="0.2"/>
-    <row r="35" x14ac:dyDescent="0.2"/>
-    <row r="36" x14ac:dyDescent="0.2"/>
-    <row r="37" x14ac:dyDescent="0.2"/>
-    <row r="38" x14ac:dyDescent="0.2"/>
-    <row r="39" x14ac:dyDescent="0.2"/>
-    <row r="40" x14ac:dyDescent="0.2"/>
-    <row r="41" x14ac:dyDescent="0.2"/>
-    <row r="42" x14ac:dyDescent="0.2"/>
-    <row r="43" x14ac:dyDescent="0.2"/>
-    <row r="44" x14ac:dyDescent="0.2"/>
-    <row r="45" x14ac:dyDescent="0.2"/>
-    <row r="46" x14ac:dyDescent="0.2"/>
-    <row r="47" x14ac:dyDescent="0.2"/>
-    <row r="48" x14ac:dyDescent="0.2"/>
+      <c r="E33" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2"/>
     <row r="49" x14ac:dyDescent="0.2"/>
     <row r="50" x14ac:dyDescent="0.2"/>
     <row r="51" x14ac:dyDescent="0.2"/>

</xml_diff>